<commit_message>
DBH Addon Expanded Pack - 3125246043 업데이트
</commit_message>
<xml_diff>
--- a/Data/DBH Addon Expanded Pack - 3125246043/3125246043_240728_00.xlsx
+++ b/Data/DBH Addon Expanded Pack - 3125246043/3125246043_240728_00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.9.1\새 폴더 (2)\DBH Addon Expanded Pack - 3125246043\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\DBH Addon Expanded Pack - 3125246043\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B219D8A-92EB-4C8D-855E-3E5ABA36DA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03F5025-660B-4E86-8E45-632B672573BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240728" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-16에 새로 추가된 노드들 (2개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{4E8B4F01-E5DC-4F47-B64E-ADAEE3206BC5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-16에 새로 추가된 노드들 (2개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -55,12 +91,27 @@
     <t>ResearchProjectDef+RoyalFixtures.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>왕실 욕실 비품</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RoyalFixtures.description</t>
   </si>
   <si>
     <t>Build luxuary bathroom fixtures like toilets, baths and basins for nobles.</t>
   </si>
   <si>
+    <t>귀족을 위한 화장실, 욕조, 세면대 등 고급스러운 욕실 비품을 제작하세요.</t>
+  </si>
+  <si>
     <t>ThingDef+DBHA_SmallWaterTank.label</t>
   </si>
   <si>
@@ -76,6 +127,18 @@
     <t>ThingDef+DBHA_WaterTank.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>물 저장고</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DBHA_WaterTank.label</t>
   </si>
   <si>
@@ -85,6 +148,18 @@
     <t>ThingDef+DBHA_HotWaterTank.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>큰 물 저장고</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DBHA_HotWaterTank.label</t>
   </si>
   <si>
@@ -94,6 +169,18 @@
     <t>ThingDef+DBHA_HotWaterTank.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>큰 온수 저장고</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DBHA_HotWaterTank.description</t>
   </si>
   <si>
@@ -103,12 +190,27 @@
     <t>ThingDef+RoyalBath.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>샤워와 목욕을 위해 뜨거운 물을 저장합니다. 난방기에 연결하여 데우세요.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RoyalBath.label</t>
   </si>
   <si>
     <t>royal bath</t>
   </si>
   <si>
+    <t>왕실 욕조</t>
+  </si>
+  <si>
     <t>ThingDef+RoyalBath.description</t>
   </si>
   <si>
@@ -121,12 +223,27 @@
     <t>ThingDef+RoyalToilet.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>사용 속도가 느리지만 매우 편안하고 아름다운 고급 욕조입니다. 인접한 캠프파이어나 통나무 보일러를 설치하거나 배관으로 연결된 온수 탱크를 통해 가열할 수 있습니다. 하수구가 필요하지 않습니다.\n매회 물 190L 사용</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RoyalToilet.label</t>
   </si>
   <si>
     <t>royal toilet</t>
   </si>
   <si>
+    <t>왕실 화장실</t>
+  </si>
+  <si>
     <t>ThingDef+RoyalToilet.description</t>
   </si>
   <si>
@@ -148,6 +265,18 @@
     <t>ThingDef+RoyalBasin.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>왕실 세면대</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RoyalBasin.description</t>
   </si>
   <si>
@@ -157,6 +286,18 @@
     <t>ThingDef+AncientBath.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>화장실 사용 후 손을 깨끗하게 씻을 수 있는 고급스러운 세면대입니다. 매우 편안하고 아름답습니다.\n매회 물 14L 사용</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>AncientBath.label</t>
   </si>
   <si>
@@ -166,6 +307,9 @@
     <t>ancient bath</t>
   </si>
   <si>
+    <t>고대 욕조</t>
+  </si>
+  <si>
     <t>ThingDef+AncientBath.description</t>
   </si>
   <si>
@@ -175,63 +319,49 @@
     <t>Slow to use, and not very comfortable. Can be heated by placing an adjacent campfire or log boiler, or via plumbed hot water tanks. Does not require a sewage outlet.\n190L per wash</t>
   </si>
   <si>
-    <t>물 저장고</t>
+    <t>ThingDef+DBHA_SmallWaterTank.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>사용 속도가 느리고 편안하지 않습니다. 인접한 캠프파이어나 통나무 보일러를 설치하거나 배관으로 연결된 온수 탱크를 통해 가열할 수 있습니다. 하수구가 필요하지 않습니다.\n매회 물 190L 사용</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>DBHA_SmallWaterTank.description</t>
+  </si>
+  <si>
+    <t>Stores water for use by plumbed fixtures. If the contained water becomes contaminated, the tank must be drained.</t>
+  </si>
+  <si>
+    <t>ThingDef+DBHA_WaterTank.description</t>
+  </si>
+  <si>
+    <t>DBHA_WaterTank.description</t>
+  </si>
+  <si>
+    <t>사람의 소변과 대변을 처리하는 데 사용되는 고급 위생 설비입니다. 높은 편안함, 매우 매력적인 - 진짜 왕좌.\n매회 물 14L 사용</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stores water for use by plumbed fixtures. If the contained water becomes contaminated, the tank must be drained.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>큰 물 저장고</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>큰 온수 저장고</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>샤워와 목욕을 위해 뜨거운 물을 저장합니다. 난방기에 연결하여 데우세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>귀족을 위한 화장실, 욕조, 세면대 등 고급스러운 욕실 비품을 제작하세요.</t>
-  </si>
-  <si>
-    <t>왕실 욕조</t>
-  </si>
-  <si>
-    <t>왕실 화장실</t>
-  </si>
-  <si>
-    <t>왕실 세면대</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>고대 욕조</t>
-  </si>
-  <si>
-    <t>사용 속도가 느리지만 매우 편안하고 아름다운 고급 욕조입니다. 인접한 캠프파이어나 통나무 보일러를 설치하거나 배관으로 연결된 온수 탱크를 통해 가열할 수 있습니다. 하수구가 필요하지 않습니다.\n매회 물 190L 사용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용 속도가 느리고 편안하지 않습니다. 인접한 캠프파이어나 통나무 보일러를 설치하거나 배관으로 연결된 온수 탱크를 통해 가열할 수 있습니다. 하수구가 필요하지 않습니다.\n매회 물 190L 사용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>화장실 사용 후 손을 깨끗하게 씻을 수 있는 고급스러운 세면대입니다. 매우 편안하고 아름답습니다.\n매회 물 14L 사용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사람의 소변과 대변을 처리하는 데 사용되는 고급 위생 설비입니다. 높은 편안함, 매우 매력적인 - 진짜 왕좌.\n매회 물 14L 사용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>왕실 욕실 비품</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>설비에서 사용될 물을 저장합니다. 저장된 물이 오염되면 배수해야합니다.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -250,13 +380,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,9 +412,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -575,11 +717,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -628,7 +770,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -639,200 +781,200 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>59</v>
@@ -840,26 +982,61 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>